<commit_message>
Added Unique Email and Username Alert
</commit_message>
<xml_diff>
--- a/se3313a-2020-lab5-testplan-lmoncad.xlsx
+++ b/se3313a-2020-lab5-testplan-lmoncad.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasmoncada/Desktop/SE-3316/se3316-lmoncad-lab5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487B2ABB-1BD3-2746-8C23-D4D103C7EB4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA03B671-C851-A54C-A591-15FBCE10B23B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{887BD6E5-E5F1-934A-BC9C-A96DFF1A2BD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1136,13 +1136,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1152,6 +1148,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1468,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96384F6-3EB5-B04C-B10F-42A7C84B59C4}">
   <dimension ref="A1:I147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E158" sqref="E158"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D146)</f>
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1561,12 +1561,12 @@
         <v>302</v>
       </c>
       <c r="D5" s="12"/>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
@@ -1575,16 +1575,16 @@
       <c r="B6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>302</v>
       </c>
       <c r="D6" s="8"/>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
@@ -1594,15 +1594,15 @@
         <v>22</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D7" s="12"/>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
@@ -1611,16 +1611,16 @@
       <c r="B8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>7</v>
+      <c r="C8" s="15" t="s">
+        <v>302</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
@@ -1630,15 +1630,15 @@
         <v>28</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
@@ -1647,7 +1647,7 @@
       <c r="B10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="15" t="s">
         <v>302</v>
       </c>
       <c r="D10" s="8"/>
@@ -1671,7 +1671,7 @@
       <c r="B12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="8"/>
@@ -1686,7 +1686,7 @@
       <c r="C13" s="11">
         <v>2</v>
       </c>
-      <c r="D13" s="18"/>
+      <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
@@ -1695,7 +1695,7 @@
       <c r="B14" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="8"/>
@@ -1719,7 +1719,7 @@
       <c r="B16" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="8"/>
@@ -1734,7 +1734,7 @@
       <c r="C17" s="11">
         <v>1</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1745,7 +1745,7 @@
       <c r="B18" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="15" t="s">
         <v>302</v>
       </c>
       <c r="D18" s="8"/>
@@ -1769,7 +1769,7 @@
       <c r="B20" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="15" t="s">
         <v>302</v>
       </c>
       <c r="D20" s="8"/>
@@ -1784,7 +1784,7 @@
       <c r="C21" s="11">
         <v>2</v>
       </c>
-      <c r="D21" s="18"/>
+      <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
@@ -1793,7 +1793,7 @@
       <c r="B22" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="8"/>
@@ -1817,7 +1817,7 @@
       <c r="B24" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="8"/>
@@ -1844,7 +1844,9 @@
       <c r="C26" s="7">
         <v>1</v>
       </c>
-      <c r="D26" s="13"/>
+      <c r="D26" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
@@ -1854,7 +1856,7 @@
         <v>65</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D27" s="12"/>
     </row>
@@ -1865,8 +1867,8 @@
       <c r="B28" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="16" t="s">
-        <v>7</v>
+      <c r="C28" s="15" t="s">
+        <v>302</v>
       </c>
       <c r="D28" s="8"/>
     </row>
@@ -1915,7 +1917,7 @@
       <c r="B32" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="15" t="s">
         <v>302</v>
       </c>
       <c r="D32" s="8"/>
@@ -1965,7 +1967,7 @@
       <c r="B36" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="15" t="s">
         <v>302</v>
       </c>
       <c r="D36" s="8"/>
@@ -1980,7 +1982,7 @@
       <c r="C37" s="11">
         <v>2</v>
       </c>
-      <c r="D37" s="18"/>
+      <c r="D37" s="16"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
@@ -1989,7 +1991,7 @@
       <c r="B38" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D38" s="8"/>
@@ -2016,7 +2018,9 @@
       <c r="C40" s="7">
         <v>4</v>
       </c>
-      <c r="D40" s="13"/>
+      <c r="D40" s="13">
+        <v>4</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
@@ -2037,7 +2041,7 @@
       <c r="B42" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="15" t="s">
         <v>302</v>
       </c>
       <c r="D42" s="8"/>
@@ -2050,7 +2054,7 @@
         <v>97</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D43" s="12"/>
     </row>
@@ -2085,7 +2089,7 @@
       <c r="B46" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C46" s="16" t="s">
+      <c r="C46" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D46" s="8"/>
@@ -2112,7 +2116,9 @@
       <c r="C48" s="7">
         <v>3</v>
       </c>
-      <c r="D48" s="13"/>
+      <c r="D48" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
@@ -2133,7 +2139,7 @@
       <c r="B50" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="15" t="s">
         <v>302</v>
       </c>
       <c r="D50" s="8"/>
@@ -2157,7 +2163,7 @@
       <c r="B52" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="C52" s="15" t="s">
         <v>302</v>
       </c>
       <c r="D52" s="8"/>
@@ -2184,7 +2190,9 @@
       <c r="C54" s="7">
         <v>1</v>
       </c>
-      <c r="D54" s="13"/>
+      <c r="D54" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
@@ -2205,7 +2213,7 @@
       <c r="B56" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C56" s="15" t="s">
         <v>302</v>
       </c>
       <c r="D56" s="8"/>
@@ -2229,7 +2237,7 @@
       <c r="B58" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="15" t="s">
         <v>302</v>
       </c>
       <c r="D58" s="8"/>
@@ -2244,7 +2252,7 @@
       <c r="C59" s="11">
         <v>3</v>
       </c>
-      <c r="D59" s="18"/>
+      <c r="D59" s="16"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
@@ -2253,7 +2261,7 @@
       <c r="B60" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C60" s="16" t="s">
+      <c r="C60" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D60" s="8"/>
@@ -2277,7 +2285,7 @@
       <c r="B62" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D62" s="8"/>
@@ -2304,7 +2312,9 @@
       <c r="C64" s="7">
         <v>10</v>
       </c>
-      <c r="D64" s="13"/>
+      <c r="D64" s="13">
+        <v>10</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
@@ -2314,7 +2324,7 @@
         <v>140</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D65" s="12"/>
     </row>
@@ -2325,8 +2335,8 @@
       <c r="B66" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C66" s="16" t="s">
-        <v>7</v>
+      <c r="C66" s="15" t="s">
+        <v>302</v>
       </c>
       <c r="D66" s="8"/>
     </row>
@@ -2338,7 +2348,7 @@
         <v>144</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D67" s="12"/>
     </row>
@@ -2349,8 +2359,8 @@
       <c r="B68" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C68" s="16" t="s">
-        <v>7</v>
+      <c r="C68" s="15" t="s">
+        <v>302</v>
       </c>
       <c r="D68" s="8"/>
     </row>
@@ -2362,7 +2372,7 @@
         <v>148</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D69" s="12"/>
     </row>
@@ -2373,8 +2383,8 @@
       <c r="B70" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C70" s="16" t="s">
-        <v>7</v>
+      <c r="C70" s="15" t="s">
+        <v>302</v>
       </c>
       <c r="D70" s="8"/>
     </row>
@@ -2388,7 +2398,7 @@
       <c r="C71" s="11">
         <v>4</v>
       </c>
-      <c r="D71" s="18"/>
+      <c r="D71" s="16"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
@@ -2397,7 +2407,7 @@
       <c r="B72" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C72" s="16" t="s">
+      <c r="C72" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D72" s="8"/>
@@ -2421,7 +2431,7 @@
       <c r="B74" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C74" s="16" t="s">
+      <c r="C74" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D74" s="8"/>
@@ -2445,7 +2455,7 @@
       <c r="B76" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C76" s="16" t="s">
+      <c r="C76" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D76" s="8"/>
@@ -2469,7 +2479,7 @@
       <c r="B78" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C78" s="16" t="s">
+      <c r="C78" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D78" s="8"/>
@@ -2493,7 +2503,7 @@
       <c r="B80" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="C80" s="16" t="s">
+      <c r="C80" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D80" s="8"/>
@@ -2508,7 +2518,9 @@
       <c r="C81" s="11">
         <v>3</v>
       </c>
-      <c r="D81" s="18"/>
+      <c r="D81" s="16">
+        <v>3</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
@@ -2517,8 +2529,8 @@
       <c r="B82" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C82" s="16" t="s">
-        <v>7</v>
+      <c r="C82" s="15" t="s">
+        <v>302</v>
       </c>
       <c r="D82" s="8"/>
     </row>
@@ -2530,7 +2542,7 @@
         <v>176</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D83" s="12"/>
     </row>
@@ -2541,8 +2553,8 @@
       <c r="B84" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="C84" s="16" t="s">
-        <v>7</v>
+      <c r="C84" s="15" t="s">
+        <v>302</v>
       </c>
       <c r="D84" s="8"/>
     </row>
@@ -2554,7 +2566,7 @@
         <v>180</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D85" s="12"/>
     </row>
@@ -2565,8 +2577,8 @@
       <c r="B86" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="C86" s="16" t="s">
-        <v>7</v>
+      <c r="C86" s="15" t="s">
+        <v>302</v>
       </c>
       <c r="D86" s="8"/>
     </row>
@@ -2580,7 +2592,7 @@
       <c r="C87" s="11">
         <v>6</v>
       </c>
-      <c r="D87" s="18"/>
+      <c r="D87" s="16"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
@@ -2589,7 +2601,7 @@
       <c r="B88" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C88" s="16" t="s">
+      <c r="C88" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D88" s="8"/>
@@ -2613,7 +2625,7 @@
       <c r="B90" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="C90" s="16" t="s">
+      <c r="C90" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D90" s="8"/>
@@ -2676,7 +2688,7 @@
       <c r="C95" s="11">
         <v>4</v>
       </c>
-      <c r="D95" s="18"/>
+      <c r="D95" s="16"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
@@ -2685,7 +2697,7 @@
       <c r="B96" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="C96" s="16" t="s">
+      <c r="C96" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D96" s="8"/>
@@ -2733,7 +2745,7 @@
       <c r="B100" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="C100" s="16" t="s">
+      <c r="C100" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D100" s="8"/>
@@ -2781,7 +2793,7 @@
       <c r="B104" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="C104" s="16" t="s">
+      <c r="C104" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D104" s="8"/>
@@ -2805,7 +2817,7 @@
       <c r="B106" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="C106" s="16" t="s">
+      <c r="C106" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D106" s="8"/>
@@ -2820,7 +2832,7 @@
       <c r="C107" s="11">
         <v>2</v>
       </c>
-      <c r="D107" s="18"/>
+      <c r="D107" s="16"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
@@ -2829,7 +2841,7 @@
       <c r="B108" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="C108" s="16" t="s">
+      <c r="C108" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D108" s="8"/>
@@ -2853,7 +2865,7 @@
       <c r="B110" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="C110" s="16" t="s">
+      <c r="C110" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D110" s="8"/>
@@ -2892,7 +2904,7 @@
       <c r="C113" s="11">
         <v>5</v>
       </c>
-      <c r="D113" s="18">
+      <c r="D113" s="16">
         <v>5</v>
       </c>
     </row>
@@ -2903,7 +2915,7 @@
       <c r="B114" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="C114" s="16" t="s">
+      <c r="C114" s="15" t="s">
         <v>302</v>
       </c>
       <c r="D114" s="8"/>
@@ -2968,7 +2980,7 @@
       <c r="C119" s="11">
         <v>2</v>
       </c>
-      <c r="D119" s="18"/>
+      <c r="D119" s="16"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="6" t="s">
@@ -2977,7 +2989,7 @@
       <c r="B120" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="C120" s="16" t="s">
+      <c r="C120" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D120" s="8"/>
@@ -3001,7 +3013,7 @@
       <c r="B122" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="C122" s="16" t="s">
+      <c r="C122" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D122" s="8"/>
@@ -3049,7 +3061,7 @@
       <c r="B126" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="C126" s="16" t="s">
+      <c r="C126" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D126" s="8"/>
@@ -3073,7 +3085,7 @@
       <c r="B128" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="C128" s="16" t="s">
+      <c r="C128" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D128" s="8"/>
@@ -3121,7 +3133,7 @@
       <c r="B132" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="C132" s="16" t="s">
+      <c r="C132" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D132" s="8"/>
@@ -3145,7 +3157,7 @@
       <c r="B134" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="C134" s="16" t="s">
+      <c r="C134" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D134" s="8"/>
@@ -3193,7 +3205,7 @@
       <c r="B138" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="C138" s="16" t="s">
+      <c r="C138" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D138" s="8"/>
@@ -3208,7 +3220,7 @@
       <c r="C139" s="11">
         <v>1</v>
       </c>
-      <c r="D139" s="18"/>
+      <c r="D139" s="16"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="6" t="s">
@@ -3217,7 +3229,7 @@
       <c r="B140" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="C140" s="16" t="s">
+      <c r="C140" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D140" s="8"/>
@@ -3241,7 +3253,7 @@
       <c r="B142" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="C142" s="16" t="s">
+      <c r="C142" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D142" s="8"/>
@@ -3256,7 +3268,7 @@
       <c r="C143" s="11">
         <v>1</v>
       </c>
-      <c r="D143" s="18"/>
+      <c r="D143" s="16"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="6" t="s">
@@ -3265,7 +3277,7 @@
       <c r="B144" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="C144" s="16" t="s">
+      <c r="C144" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D144" s="8"/>
@@ -3280,19 +3292,19 @@
       <c r="C145" s="11">
         <v>1</v>
       </c>
-      <c r="D145" s="18"/>
+      <c r="D145" s="16"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A146" s="19" t="s">
+      <c r="A146" s="17" t="s">
         <v>300</v>
       </c>
-      <c r="B146" s="20" t="s">
+      <c r="B146" s="18" t="s">
         <v>301</v>
       </c>
-      <c r="C146" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D146" s="22"/>
+      <c r="C146" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D146" s="20"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C147">
@@ -3301,7 +3313,7 @@
       </c>
       <c r="D147">
         <f>SUM(D2:D146)</f>
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added logging out feature
</commit_message>
<xml_diff>
--- a/se3313a-2020-lab5-testplan-lmoncad.xlsx
+++ b/se3313a-2020-lab5-testplan-lmoncad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasmoncada/Desktop/SE-3316/se3316-lmoncad-lab5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA03B671-C851-A54C-A591-15FBCE10B23B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBE106F-1890-464F-B5A9-2BFB843AB893}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{887BD6E5-E5F1-934A-BC9C-A96DFF1A2BD9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="303">
   <si>
     <t>ID</t>
   </si>
@@ -1468,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96384F6-3EB5-B04C-B10F-42A7C84B59C4}">
   <dimension ref="A1:I147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D146)</f>
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1548,7 +1548,9 @@
       <c r="C4" s="7">
         <v>4</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="13">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
@@ -1672,7 +1674,7 @@
         <v>35</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D12" s="8"/>
     </row>
@@ -1695,9 +1697,7 @@
       <c r="B14" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>7</v>
-      </c>
+      <c r="C14" s="15"/>
       <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2688,7 +2688,9 @@
       <c r="C95" s="11">
         <v>4</v>
       </c>
-      <c r="D95" s="16"/>
+      <c r="D95" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
@@ -2698,7 +2700,7 @@
         <v>202</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D96" s="8"/>
     </row>
@@ -2710,7 +2712,7 @@
         <v>204</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D97" s="12"/>
     </row>
@@ -2832,7 +2834,9 @@
       <c r="C107" s="11">
         <v>2</v>
       </c>
-      <c r="D107" s="16"/>
+      <c r="D107" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
@@ -2842,7 +2846,7 @@
         <v>226</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D108" s="8"/>
     </row>
@@ -2854,7 +2858,7 @@
         <v>228</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D109" s="12"/>
     </row>
@@ -2866,7 +2870,7 @@
         <v>230</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D110" s="8"/>
     </row>
@@ -2878,7 +2882,7 @@
         <v>232</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D111" s="12"/>
     </row>
@@ -3313,7 +3317,7 @@
       </c>
       <c r="D147">
         <f>SUM(D2:D146)</f>
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Displaying Current User's Course Lists
</commit_message>
<xml_diff>
--- a/se3313a-2020-lab5-testplan-lmoncad.xlsx
+++ b/se3313a-2020-lab5-testplan-lmoncad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasmoncada/Desktop/SE-3316/se3316-lmoncad-lab5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97CFBEC-E6B2-6348-97A9-CB2B81B45B78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC65668-EE9D-4D48-A0BF-921AFEB0263A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{887BD6E5-E5F1-934A-BC9C-A96DFF1A2BD9}"/>
   </bookViews>
@@ -1468,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96384F6-3EB5-B04C-B10F-42A7C84B59C4}">
   <dimension ref="A1:I147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D146)</f>
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2728,7 +2728,9 @@
       <c r="C98" s="7">
         <v>2</v>
       </c>
-      <c r="D98" s="13"/>
+      <c r="D98" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
@@ -2750,7 +2752,7 @@
         <v>210</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D100" s="8"/>
     </row>
@@ -2762,7 +2764,7 @@
         <v>212</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D101" s="12"/>
     </row>
@@ -3321,7 +3323,7 @@
       </c>
       <c r="D147">
         <f>SUM(D2:D146)</f>
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Editing Course and Fixed Number of Course Bug
</commit_message>
<xml_diff>
--- a/se3313a-2020-lab5-testplan-lmoncad.xlsx
+++ b/se3313a-2020-lab5-testplan-lmoncad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasmoncada/Desktop/SE-3316/se3316-lmoncad-lab5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC65668-EE9D-4D48-A0BF-921AFEB0263A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E4E6E9-5343-974C-9402-E5ED0F7274B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{887BD6E5-E5F1-934A-BC9C-A96DFF1A2BD9}"/>
   </bookViews>
@@ -1468,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96384F6-3EB5-B04C-B10F-42A7C84B59C4}">
   <dimension ref="A1:I147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B139" sqref="B139"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2408,7 +2408,7 @@
         <v>154</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D72" s="8"/>
     </row>

</xml_diff>

<commit_message>
Added Timetable Displaying of Course Lists
</commit_message>
<xml_diff>
--- a/se3313a-2020-lab5-testplan-lmoncad.xlsx
+++ b/se3313a-2020-lab5-testplan-lmoncad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasmoncada/Desktop/SE-3316/se3316-lmoncad-lab5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E4E6E9-5343-974C-9402-E5ED0F7274B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411907C1-BEDE-7849-8F34-4144713DDE93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{887BD6E5-E5F1-934A-BC9C-A96DFF1A2BD9}"/>
+    <workbookView xWindow="8740" yWindow="6760" windowWidth="27640" windowHeight="16940" xr2:uid="{887BD6E5-E5F1-934A-BC9C-A96DFF1A2BD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="303">
   <si>
     <t>ID</t>
   </si>
@@ -1468,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96384F6-3EB5-B04C-B10F-42A7C84B59C4}">
   <dimension ref="A1:I147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D146)</f>
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1511,9 +1511,7 @@
       <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>302</v>
-      </c>
+      <c r="C2" s="7"/>
       <c r="D2" s="8"/>
       <c r="F2" s="4" t="s">
         <v>8</v>
@@ -2252,7 +2250,9 @@
       <c r="C59" s="11">
         <v>3</v>
       </c>
-      <c r="D59" s="16"/>
+      <c r="D59" s="16">
+        <v>3</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
@@ -2262,7 +2262,7 @@
         <v>131</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D60" s="8"/>
     </row>
@@ -2274,7 +2274,7 @@
         <v>125</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D61" s="12"/>
     </row>
@@ -2286,7 +2286,7 @@
         <v>134</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D62" s="8"/>
     </row>
@@ -2398,7 +2398,9 @@
       <c r="C71" s="11">
         <v>4</v>
       </c>
-      <c r="D71" s="16"/>
+      <c r="D71" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
@@ -2420,7 +2422,7 @@
         <v>156</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D73" s="12"/>
     </row>
@@ -2432,7 +2434,7 @@
         <v>158</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D74" s="8"/>
     </row>
@@ -2444,7 +2446,7 @@
         <v>160</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D75" s="12"/>
     </row>
@@ -2456,7 +2458,7 @@
         <v>162</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D76" s="8"/>
     </row>
@@ -2468,7 +2470,7 @@
         <v>164</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D77" s="12"/>
     </row>
@@ -2480,7 +2482,7 @@
         <v>166</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D78" s="8"/>
     </row>
@@ -2492,7 +2494,7 @@
         <v>168</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D79" s="12"/>
     </row>
@@ -2504,7 +2506,7 @@
         <v>170</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D80" s="8"/>
     </row>
@@ -2654,7 +2656,9 @@
       <c r="C92" s="7">
         <v>2</v>
       </c>
-      <c r="D92" s="13"/>
+      <c r="D92" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
@@ -2664,7 +2668,7 @@
         <v>196</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D93" s="12"/>
     </row>
@@ -3323,7 +3327,7 @@
       </c>
       <c r="D147">
         <f>SUM(D2:D146)</f>
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Full Copyright Functionality
</commit_message>
<xml_diff>
--- a/se3313a-2020-lab5-testplan-lmoncad.xlsx
+++ b/se3313a-2020-lab5-testplan-lmoncad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasmoncada/Desktop/SE-3316/se3316-lmoncad-lab5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411907C1-BEDE-7849-8F34-4144713DDE93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1A677E-1A9D-6F47-922E-915E0853F83C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8740" yWindow="6760" windowWidth="27640" windowHeight="16940" xr2:uid="{887BD6E5-E5F1-934A-BC9C-A96DFF1A2BD9}"/>
   </bookViews>
@@ -1468,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96384F6-3EB5-B04C-B10F-42A7C84B59C4}">
   <dimension ref="A1:I147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D146)</f>
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1980,7 +1980,9 @@
       <c r="C37" s="11">
         <v>2</v>
       </c>
-      <c r="D37" s="16"/>
+      <c r="D37" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
@@ -1990,7 +1992,7 @@
         <v>87</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D38" s="8"/>
     </row>
@@ -3327,7 +3329,7 @@
       </c>
       <c r="D147">
         <f>SUM(D2:D146)</f>
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some more comments
</commit_message>
<xml_diff>
--- a/se3313a-2020-lab5-testplan-lmoncad.xlsx
+++ b/se3313a-2020-lab5-testplan-lmoncad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasmoncada/Desktop/SE-3316/se3316-lmoncad-lab5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1A677E-1A9D-6F47-922E-915E0853F83C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD0DF9C-99EF-6243-B266-BB4CE0E9BED3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8740" yWindow="6760" windowWidth="27640" windowHeight="16940" xr2:uid="{887BD6E5-E5F1-934A-BC9C-A96DFF1A2BD9}"/>
+    <workbookView xWindow="3720" yWindow="5480" windowWidth="37560" windowHeight="20160" xr2:uid="{887BD6E5-E5F1-934A-BC9C-A96DFF1A2BD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1468,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96384F6-3EB5-B04C-B10F-42A7C84B59C4}">
   <dimension ref="A1:I147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="G1" s="5">
         <f>SUM(D2:D146)</f>
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2996,7 +2996,9 @@
       <c r="C119" s="11">
         <v>2</v>
       </c>
-      <c r="D119" s="16"/>
+      <c r="D119" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="6" t="s">
@@ -3006,7 +3008,7 @@
         <v>250</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D120" s="8"/>
     </row>
@@ -3018,7 +3020,7 @@
         <v>252</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D121" s="12"/>
     </row>
@@ -3030,7 +3032,7 @@
         <v>254</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D122" s="8"/>
     </row>
@@ -3042,7 +3044,7 @@
         <v>256</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D123" s="12"/>
     </row>
@@ -3056,7 +3058,9 @@
       <c r="C124" s="7">
         <v>2</v>
       </c>
-      <c r="D124" s="13"/>
+      <c r="D124" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="10" t="s">
@@ -3066,7 +3070,7 @@
         <v>260</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D125" s="12"/>
     </row>
@@ -3078,7 +3082,7 @@
         <v>262</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D126" s="8"/>
     </row>
@@ -3090,7 +3094,7 @@
         <v>264</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D127" s="12"/>
     </row>
@@ -3102,7 +3106,7 @@
         <v>266</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D128" s="8"/>
     </row>
@@ -3114,7 +3118,7 @@
         <v>256</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D129" s="12"/>
     </row>
@@ -3128,7 +3132,9 @@
       <c r="C130" s="7">
         <v>2</v>
       </c>
-      <c r="D130" s="13"/>
+      <c r="D130" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
@@ -3138,7 +3144,7 @@
         <v>271</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D131" s="12"/>
     </row>
@@ -3150,7 +3156,7 @@
         <v>273</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D132" s="8"/>
     </row>
@@ -3162,7 +3168,7 @@
         <v>275</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D133" s="12"/>
     </row>
@@ -3174,7 +3180,7 @@
         <v>277</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D134" s="8"/>
     </row>
@@ -3186,7 +3192,7 @@
         <v>279</v>
       </c>
       <c r="C135" s="11" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="D135" s="12"/>
     </row>
@@ -3329,7 +3335,7 @@
       </c>
       <c r="D147">
         <f>SUM(D2:D146)</f>
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed links to the correct address for new ec2 instance
</commit_message>
<xml_diff>
--- a/se3313a-2020-lab5-testplan-lmoncad.xlsx
+++ b/se3313a-2020-lab5-testplan-lmoncad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasmoncada/Desktop/SE-3316/se3316-lmoncad-lab5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD0DF9C-99EF-6243-B266-BB4CE0E9BED3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C125459C-7FE7-7943-8A8E-1D17146FA000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3720" yWindow="5480" windowWidth="37560" windowHeight="20160" xr2:uid="{887BD6E5-E5F1-934A-BC9C-A96DFF1A2BD9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="304">
   <si>
     <t>ID</t>
   </si>
@@ -943,13 +943,16 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>5e94ac6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -961,6 +964,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1108,10 +1119,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1152,8 +1164,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1469,7 +1483,7 @@
   <dimension ref="A1:I147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="F5" sqref="F5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1534,7 +1548,9 @@
       <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="23" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
@@ -3346,6 +3362,10 @@
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="F9:I9"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" display="https://github.com/lucasmoncada08/se3316-lmoncad-lab5/commit/5e94ac6964e297a3ac397d9601347e5e8851d209" xr:uid="{82318D40-BA72-4646-82FD-4F481D12D019}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>